<commit_message>
now finished adding the word document class. Now working to get client name and then convert the word doc to pdf
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>Product Name</t>
   </si>
@@ -28,7 +28,10 @@
     <t>Total</t>
   </si>
   <si>
-    <t>Air pods</t>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
   </si>
   <si>
     <t>Sub Total</t>
@@ -366,7 +369,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -391,21 +394,27 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>150</v>
+        <v>1</v>
       </c>
       <c r="C3">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>15000</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>5</v>
       </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
       <c r="D4">
-        <v>15000</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -413,15 +422,23 @@
         <v>6</v>
       </c>
       <c r="D5">
-        <v>1950</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
         <v>3</v>
       </c>
-      <c r="D6">
-        <v>16950</v>
+      <c r="D7">
+        <v>5.65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>